<commit_message>
Added Logging and Open/Close to XXXAction
</commit_message>
<xml_diff>
--- a/VNCPhidget22/AppStartupTrace.xlsx
+++ b/VNCPhidget22/AppStartupTrace.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\chrhodes\VNCPhidgets\VNCPhidget22\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC223EF-D6B6-4D16-A1FE-0C4A34887122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F05843F-34D4-4E0A-B10A-DFD75A3B739D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32300" yWindow="3780" windowWidth="28800" windowHeight="15450" xr2:uid="{52DEDB99-C28F-4341-B0F2-851AB361A74E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{52DEDB99-C28F-4341-B0F2-851AB361A74E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>

</xml_diff>